<commit_message>
Fix input data reference errors
</commit_message>
<xml_diff>
--- a/InputData/elec/BCpUC/Battery Cost per Unit Cap.xlsx
+++ b/InputData/elec/BCpUC/Battery Cost per Unit Cap.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\elec\BCpUC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-oregon\InputData\elec\BCpUC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26C6F2EA-4A60-4C7E-ADE8-36917C57C687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD83BBC7-696E-4685-844D-838E6579DF9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="BCpUC" sheetId="3" r:id="rId5"/>
     <sheet name="BBoSCpUC" sheetId="4" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -2329,22 +2329,22 @@
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="67.1796875" customWidth="1"/>
+    <col min="2" max="2" width="67.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -2352,198 +2352,198 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="4">
         <v>2014</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B13" s="4">
         <v>2013</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="18" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="19" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B19" s="8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="4">
         <v>2021</v>
       </c>
     </row>
-    <row r="21" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="22" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="8" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="25" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="4">
         <v>2018</v>
       </c>
     </row>
-    <row r="28" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="8" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="36" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
     </row>
-    <row r="37" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="38" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="39" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="40" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="41" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5"/>
     </row>
-    <row r="42" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="43" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="44" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="45" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="5"/>
     </row>
-    <row r="46" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="8">
         <v>1.0549999999999999</v>
       </c>
@@ -2551,7 +2551,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="49" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="43">
         <v>0.9143273584567535</v>
       </c>
@@ -2559,7 +2559,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
         <v>15</v>
       </c>
@@ -2582,17 +2582,17 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="33.36328125" customWidth="1"/>
+    <col min="5" max="5" width="33.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:37" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:37" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="2:37" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:37" x14ac:dyDescent="0.25">
       <c r="F2">
         <v>2019</v>
       </c>
@@ -2690,7 +2690,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="3" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>70</v>
       </c>
@@ -2797,7 +2797,7 @@
         <v>205.4624</v>
       </c>
     </row>
-    <row r="4" spans="2:37" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:37" x14ac:dyDescent="0.25">
       <c r="E4" t="s">
         <v>73</v>
       </c>
@@ -2898,7 +2898,7 @@
         <v>384.774771419959</v>
       </c>
     </row>
-    <row r="5" spans="2:37" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:37" x14ac:dyDescent="0.25">
       <c r="E5" t="s">
         <v>74</v>
       </c>
@@ -2999,7 +2999,7 @@
         <v>594.1617</v>
       </c>
     </row>
-    <row r="6" spans="2:37" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:37" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
         <v>75</v>
       </c>
@@ -3100,7 +3100,7 @@
         <v>345.73</v>
       </c>
     </row>
-    <row r="7" spans="2:37" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:37" x14ac:dyDescent="0.25">
       <c r="E7" t="s">
         <v>76</v>
       </c>
@@ -3201,7 +3201,7 @@
         <v>588.07036627634386</v>
       </c>
     </row>
-    <row r="8" spans="2:37" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:37" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
         <v>77</v>
       </c>
@@ -3302,7 +3302,7 @@
         <v>980.8854</v>
       </c>
     </row>
-    <row r="9" spans="2:37" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:37" x14ac:dyDescent="0.25">
       <c r="E9" t="s">
         <v>78</v>
       </c>
@@ -3403,7 +3403,7 @@
         <v>485.99760000000003</v>
       </c>
     </row>
-    <row r="10" spans="2:37" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:37" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
         <v>79</v>
       </c>
@@ -3504,7 +3504,7 @@
         <v>791.36596113272867</v>
       </c>
     </row>
-    <row r="11" spans="2:37" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:37" x14ac:dyDescent="0.25">
       <c r="E11" t="s">
         <v>80</v>
       </c>
@@ -3605,7 +3605,7 @@
         <v>1367.6091000000001</v>
       </c>
     </row>
-    <row r="12" spans="2:37" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:37" x14ac:dyDescent="0.25">
       <c r="E12" t="s">
         <v>81</v>
       </c>
@@ -3706,7 +3706,7 @@
         <v>626.26520000000005</v>
       </c>
     </row>
-    <row r="13" spans="2:37" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:37" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
         <v>82</v>
       </c>
@@ -3807,7 +3807,7 @@
         <v>994.66155598911359</v>
       </c>
     </row>
-    <row r="14" spans="2:37" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:37" x14ac:dyDescent="0.25">
       <c r="E14" t="s">
         <v>83</v>
       </c>
@@ -3908,7 +3908,7 @@
         <v>1754.3328000000001</v>
       </c>
     </row>
-    <row r="15" spans="2:37" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:37" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
         <v>84</v>
       </c>
@@ -4009,7 +4009,7 @@
         <v>766.53280000000007</v>
       </c>
     </row>
-    <row r="16" spans="2:37" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:37" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
         <v>85</v>
       </c>
@@ -4110,7 +4110,7 @@
         <v>1197.9571508454985</v>
       </c>
     </row>
-    <row r="17" spans="5:37" x14ac:dyDescent="0.35">
+    <row r="17" spans="5:37" x14ac:dyDescent="0.25">
       <c r="E17" t="s">
         <v>86</v>
       </c>
@@ -4224,14 +4224,14 @@
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.54296875" style="10" customWidth="1"/>
-    <col min="2" max="13" width="11.26953125" style="10" customWidth="1"/>
-    <col min="14" max="16384" width="9.1796875" style="10"/>
+    <col min="1" max="1" width="32.5703125" style="10" customWidth="1"/>
+    <col min="2" max="13" width="11.28515625" style="10" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="36" t="s">
         <v>23</v>
       </c>
@@ -4248,7 +4248,7 @@
       <c r="L1" s="37"/>
       <c r="M1" s="37"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="19"/>
       <c r="B2" s="46" t="s">
         <v>24</v>
@@ -4271,7 +4271,7 @@
       <c r="L2" s="50"/>
       <c r="M2" s="51"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
         <v>45</v>
       </c>
@@ -4312,7 +4312,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>28</v>
       </c>
@@ -4353,7 +4353,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>29</v>
       </c>
@@ -4394,7 +4394,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>30</v>
       </c>
@@ -4435,7 +4435,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>31</v>
       </c>
@@ -4476,7 +4476,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>46</v>
       </c>
@@ -4517,7 +4517,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>32</v>
       </c>
@@ -4558,7 +4558,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>33</v>
       </c>
@@ -4599,7 +4599,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="26" t="s">
         <v>34</v>
       </c>
@@ -4640,7 +4640,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
         <v>35</v>
       </c>
@@ -4681,7 +4681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>36</v>
       </c>
@@ -4722,7 +4722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
         <v>37</v>
       </c>
@@ -4763,7 +4763,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
         <v>38</v>
       </c>
@@ -4804,7 +4804,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
         <v>39</v>
       </c>
@@ -4845,7 +4845,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>40</v>
       </c>
@@ -4886,7 +4886,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="31" t="s">
         <v>41</v>
       </c>
@@ -4927,12 +4927,12 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="38" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>56</v>
       </c>
@@ -4944,7 +4944,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="40" t="s">
         <v>57</v>
       </c>
@@ -4956,7 +4956,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="40" t="s">
         <v>22</v>
       </c>
@@ -4968,7 +4968,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="40" t="s">
         <v>22</v>
       </c>
@@ -4980,7 +4980,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="40" t="s">
         <v>22</v>
       </c>
@@ -4992,7 +4992,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
         <v>68</v>
       </c>
@@ -5017,22 +5017,22 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.81640625" style="8" customWidth="1"/>
-    <col min="2" max="2" width="26.26953125" style="8" customWidth="1"/>
-    <col min="3" max="6" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.85546875" style="8" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" style="8" customWidth="1"/>
+    <col min="3" max="6" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="19" max="21" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="22" max="32" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="21" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="32" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -5130,7 +5130,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>91</v>
       </c>
@@ -5259,12 +5259,12 @@
         <v>588070.36627634382</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>93</v>
       </c>
@@ -5362,7 +5362,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>94</v>
       </c>
@@ -5460,7 +5460,7 @@
         <v>662505</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>95</v>
       </c>
@@ -5589,7 +5589,7 @@
         <v>-74434.633723656181</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>96</v>
       </c>
@@ -5605,19 +5605,19 @@
   <sheetPr>
     <tabColor rgb="FF003399"/>
   </sheetPr>
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1048576"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.1796875" customWidth="1"/>
-    <col min="2" max="2" width="21.453125" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -5625,293 +5625,284 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>2019</v>
-      </c>
-      <c r="B2" s="6" t="e">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="8">
+        <v>2020</v>
+      </c>
+      <c r="B2" s="6">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(BCpUC!A2,'NREL ATB'!$2:$2,0))*1000-INDEX(BBoSCpUC!$2:$2,MATCH(A2,BBoSCpUC!$1:$1,0))</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+        <v>813519.89556063944</v>
+      </c>
+      <c r="E2" s="6"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="B3" s="6">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(BCpUC!A3,'NREL ATB'!$2:$2,0))*1000-INDEX(BBoSCpUC!$2:$2,MATCH(A3,BBoSCpUC!$1:$1,0))</f>
-        <v>813519.89556063944</v>
-      </c>
-      <c r="E3" s="6"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+        <v>670249.89556063944</v>
+      </c>
+      <c r="G3" s="6"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B4" s="6">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(BCpUC!A4,'NREL ATB'!$2:$2,0))*1000-INDEX(BBoSCpUC!$2:$2,MATCH(A4,BBoSCpUC!$1:$1,0))</f>
-        <v>670249.89556063944</v>
-      </c>
-      <c r="G4" s="6"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+        <v>575519.89556063944</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="B5" s="6">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(BCpUC!A5,'NREL ATB'!$2:$2,0))*1000-INDEX(BBoSCpUC!$2:$2,MATCH(A5,BBoSCpUC!$1:$1,0))</f>
-        <v>575519.89556063944</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+        <v>505619.89556063944</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B6" s="6">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(BCpUC!A6,'NREL ATB'!$2:$2,0))*1000-INDEX(BBoSCpUC!$2:$2,MATCH(A6,BBoSCpUC!$1:$1,0))</f>
-        <v>505619.89556063944</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+        <v>450056.89556063944</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="B7" s="6">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(BCpUC!A7,'NREL ATB'!$2:$2,0))*1000-INDEX(BBoSCpUC!$2:$2,MATCH(A7,BBoSCpUC!$1:$1,0))</f>
-        <v>450056.89556063944</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+        <v>405016.89556063944</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="B8" s="6">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(BCpUC!A8,'NREL ATB'!$2:$2,0))*1000-INDEX(BBoSCpUC!$2:$2,MATCH(A8,BBoSCpUC!$1:$1,0))</f>
-        <v>405016.89556063944</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+        <v>365985.89556063944</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
-        <v>2026</v>
+        <v>2027</v>
       </c>
       <c r="B9" s="6">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(BCpUC!A9,'NREL ATB'!$2:$2,0))*1000-INDEX(BBoSCpUC!$2:$2,MATCH(A9,BBoSCpUC!$1:$1,0))</f>
-        <v>365985.89556063944</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+        <v>332129.89556063944</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
-        <v>2027</v>
+        <v>2028</v>
       </c>
       <c r="B10" s="6">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(BCpUC!A10,'NREL ATB'!$2:$2,0))*1000-INDEX(BBoSCpUC!$2:$2,MATCH(A10,BBoSCpUC!$1:$1,0))</f>
-        <v>332129.89556063944</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+        <v>302999.89556063944</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
-        <v>2028</v>
+        <v>2029</v>
       </c>
       <c r="B11" s="6">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(BCpUC!A11,'NREL ATB'!$2:$2,0))*1000-INDEX(BBoSCpUC!$2:$2,MATCH(A11,BBoSCpUC!$1:$1,0))</f>
-        <v>302999.89556063944</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+        <v>277998.89556063944</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
-        <v>2029</v>
+        <v>2030</v>
       </c>
       <c r="B12" s="6">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(BCpUC!A12,'NREL ATB'!$2:$2,0))*1000-INDEX(BBoSCpUC!$2:$2,MATCH(A12,BBoSCpUC!$1:$1,0))</f>
-        <v>277998.89556063944</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+        <v>256485.89556063944</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
-        <v>2030</v>
+        <v>2031</v>
       </c>
       <c r="B13" s="6">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(BCpUC!A13,'NREL ATB'!$2:$2,0))*1000-INDEX(BBoSCpUC!$2:$2,MATCH(A13,BBoSCpUC!$1:$1,0))</f>
-        <v>256485.89556063944</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+        <v>237801.89556063944</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
-        <v>2031</v>
+        <v>2032</v>
       </c>
       <c r="B14" s="6">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(BCpUC!A14,'NREL ATB'!$2:$2,0))*1000-INDEX(BBoSCpUC!$2:$2,MATCH(A14,BBoSCpUC!$1:$1,0))</f>
-        <v>237801.89556063944</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+        <v>221749.89556063944</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
-        <v>2032</v>
+        <v>2033</v>
       </c>
       <c r="B15" s="6">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(BCpUC!A15,'NREL ATB'!$2:$2,0))*1000-INDEX(BBoSCpUC!$2:$2,MATCH(A15,BBoSCpUC!$1:$1,0))</f>
-        <v>221749.89556063944</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+        <v>208002.89556063944</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
-        <v>2033</v>
+        <v>2034</v>
       </c>
       <c r="B16" s="6">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(BCpUC!A16,'NREL ATB'!$2:$2,0))*1000-INDEX(BBoSCpUC!$2:$2,MATCH(A16,BBoSCpUC!$1:$1,0))</f>
-        <v>208002.89556063944</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+        <v>196105.89556063944</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
-        <v>2034</v>
+        <v>2035</v>
       </c>
       <c r="B17" s="6">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(BCpUC!A17,'NREL ATB'!$2:$2,0))*1000-INDEX(BBoSCpUC!$2:$2,MATCH(A17,BBoSCpUC!$1:$1,0))</f>
-        <v>196105.89556063944</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+        <v>185660.89556063944</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
-        <v>2035</v>
+        <v>2036</v>
       </c>
       <c r="B18" s="6">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(BCpUC!A18,'NREL ATB'!$2:$2,0))*1000-INDEX(BBoSCpUC!$2:$2,MATCH(A18,BBoSCpUC!$1:$1,0))</f>
-        <v>185660.89556063944</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+        <v>176492.89556063944</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
-        <v>2036</v>
+        <v>2037</v>
       </c>
       <c r="B19" s="6">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(BCpUC!A19,'NREL ATB'!$2:$2,0))*1000-INDEX(BBoSCpUC!$2:$2,MATCH(A19,BBoSCpUC!$1:$1,0))</f>
-        <v>176492.89556063944</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+        <v>168432.89556063944</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
-        <v>2037</v>
+        <v>2038</v>
       </c>
       <c r="B20" s="6">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(BCpUC!A20,'NREL ATB'!$2:$2,0))*1000-INDEX(BBoSCpUC!$2:$2,MATCH(A20,BBoSCpUC!$1:$1,0))</f>
-        <v>168432.89556063944</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+        <v>161272.89556063944</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
-        <v>2038</v>
+        <v>2039</v>
       </c>
       <c r="B21" s="6">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(BCpUC!A21,'NREL ATB'!$2:$2,0))*1000-INDEX(BBoSCpUC!$2:$2,MATCH(A21,BBoSCpUC!$1:$1,0))</f>
-        <v>161272.89556063944</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+        <v>154834.89556063944</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
-        <v>2039</v>
+        <v>2040</v>
       </c>
       <c r="B22" s="6">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(BCpUC!A22,'NREL ATB'!$2:$2,0))*1000-INDEX(BBoSCpUC!$2:$2,MATCH(A22,BBoSCpUC!$1:$1,0))</f>
-        <v>154834.89556063944</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+        <v>148994.89556063944</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
-        <v>2040</v>
+        <v>2041</v>
       </c>
       <c r="B23" s="6">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(BCpUC!A23,'NREL ATB'!$2:$2,0))*1000-INDEX(BBoSCpUC!$2:$2,MATCH(A23,BBoSCpUC!$1:$1,0))</f>
-        <v>148994.89556063944</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+        <v>143757.89556063944</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
-        <v>2041</v>
+        <v>2042</v>
       </c>
       <c r="B24" s="6">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(BCpUC!A24,'NREL ATB'!$2:$2,0))*1000-INDEX(BBoSCpUC!$2:$2,MATCH(A24,BBoSCpUC!$1:$1,0))</f>
-        <v>143757.89556063944</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+        <v>139018.89556063944</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
-        <v>2042</v>
+        <v>2043</v>
       </c>
       <c r="B25" s="6">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(BCpUC!A25,'NREL ATB'!$2:$2,0))*1000-INDEX(BBoSCpUC!$2:$2,MATCH(A25,BBoSCpUC!$1:$1,0))</f>
-        <v>139018.89556063944</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+        <v>134714.89556063944</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="8">
-        <v>2043</v>
+        <v>2044</v>
       </c>
       <c r="B26" s="6">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(BCpUC!A26,'NREL ATB'!$2:$2,0))*1000-INDEX(BBoSCpUC!$2:$2,MATCH(A26,BBoSCpUC!$1:$1,0))</f>
-        <v>134714.89556063944</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+        <v>130781.89556063944</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="8">
-        <v>2044</v>
+        <v>2045</v>
       </c>
       <c r="B27" s="6">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(BCpUC!A27,'NREL ATB'!$2:$2,0))*1000-INDEX(BBoSCpUC!$2:$2,MATCH(A27,BBoSCpUC!$1:$1,0))</f>
-        <v>130781.89556063944</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+        <v>127169.89556063944</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="8">
-        <v>2045</v>
+        <v>2046</v>
       </c>
       <c r="B28" s="6">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(BCpUC!A28,'NREL ATB'!$2:$2,0))*1000-INDEX(BBoSCpUC!$2:$2,MATCH(A28,BBoSCpUC!$1:$1,0))</f>
-        <v>127169.89556063944</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+        <v>123846.89556063944</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="8">
-        <v>2046</v>
+        <v>2047</v>
       </c>
       <c r="B29" s="6">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(BCpUC!A29,'NREL ATB'!$2:$2,0))*1000-INDEX(BBoSCpUC!$2:$2,MATCH(A29,BBoSCpUC!$1:$1,0))</f>
-        <v>123846.89556063944</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+        <v>120770.89556063944</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="8">
-        <v>2047</v>
+        <v>2048</v>
       </c>
       <c r="B30" s="6">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(BCpUC!A30,'NREL ATB'!$2:$2,0))*1000-INDEX(BBoSCpUC!$2:$2,MATCH(A30,BBoSCpUC!$1:$1,0))</f>
-        <v>120770.89556063944</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+        <v>117909.89556063944</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="8">
-        <v>2048</v>
+        <v>2049</v>
       </c>
       <c r="B31" s="6">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(BCpUC!A31,'NREL ATB'!$2:$2,0))*1000-INDEX(BBoSCpUC!$2:$2,MATCH(A31,BBoSCpUC!$1:$1,0))</f>
-        <v>117909.89556063944</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+        <v>115242.89556063944</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="8">
-        <v>2049</v>
+        <v>2050</v>
       </c>
       <c r="B32" s="6">
         <f>INDEX('NREL ATB'!$7:$7,MATCH(BCpUC!A32,'NREL ATB'!$2:$2,0))*1000-INDEX(BBoSCpUC!$2:$2,MATCH(A32,BBoSCpUC!$1:$1,0))</f>
-        <v>115242.89556063944</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A33" s="8">
-        <v>2050</v>
-      </c>
-      <c r="B33" s="6">
-        <f>INDEX('NREL ATB'!$7:$7,MATCH(BCpUC!A33,'NREL ATB'!$2:$2,0))*1000-INDEX(BBoSCpUC!$2:$2,MATCH(A33,BBoSCpUC!$1:$1,0))</f>
         <v>112744.89556063944</v>
       </c>
     </row>
@@ -5931,12 +5922,12 @@
       <selection activeCell="B2" sqref="B2:AF2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.81640625" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -6034,7 +6025,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>

</xml_diff>